<commit_message>
bổ sung chức năng
</commit_message>
<xml_diff>
--- a/Face-Recogntion-PyQt/Face_Detection_PyQt_Final/242EIE501902.xlsx
+++ b/Face-Recogntion-PyQt/Face_Detection_PyQt_Final/242EIE501902.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="14795"/>
+    <workbookView windowWidth="18744" windowHeight="15240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
   <si>
     <t>K234111385</t>
   </si>
@@ -135,12 +141,6 @@
   </si>
   <si>
     <t>Trần Khánh Linh</t>
-  </si>
-  <si>
-    <t>K234111437</t>
-  </si>
-  <si>
-    <t>Trần Khánh Ly</t>
   </si>
   <si>
     <t>K234111439</t>
@@ -261,7 +261,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,12 +277,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -626,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -635,62 +629,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -812,137 +761,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,22 +901,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1503,10 +1440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1516,307 +1453,299 @@
     <col min="3" max="16384" width="8.88888888888889" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.35" spans="1:2">
+    <row r="1" ht="15.6" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="16.35" spans="1:2">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.6" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="16.35" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="15.6" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="16.35" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="15.6" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="16.35" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15.6" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="16.35" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="15.6" spans="1:2">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="16.35" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" ht="15.6" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="16.35" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="15.6" spans="1:2">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="16.35" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" ht="15.6" spans="1:2">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="16.35" spans="1:2">
-      <c r="A10" s="5" t="s">
+    <row r="10" ht="15.6" spans="1:2">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="16.35" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" ht="15.6" spans="1:2">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="16.35" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" ht="15.6" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="16.35" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" ht="15.6" spans="1:2">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="16.35" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" ht="15.6" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="16.35" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="15" ht="15.6" spans="1:2">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="16.35" spans="1:2">
-      <c r="A16" s="3" t="s">
+    <row r="16" ht="15.6" spans="1:2">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="16.35" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="17" ht="15.6" spans="1:2">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="16.35" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" ht="15.6" spans="1:2">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="16.35" spans="1:2">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
+    <row r="19" ht="15.6" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" ht="16.35" spans="1:2">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" ht="15.6" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" ht="16.35" spans="1:2">
-      <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" ht="15.6" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" ht="16.35" spans="1:2">
-      <c r="A22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" ht="15.6" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" ht="16.35" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" ht="15.6" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" ht="16.35" spans="1:2">
-      <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" ht="15.6" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" ht="16.35" spans="1:2">
-      <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" ht="15.6" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" ht="14.55" spans="1:2">
-      <c r="A26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" ht="16.35" spans="1:2">
-      <c r="A27" s="3" t="s">
+    <row r="26" ht="15.6" spans="1:2">
+      <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" ht="15.6" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="B27" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" ht="16.35" spans="1:2">
-      <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" ht="15.6" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" ht="16.35" spans="1:2">
-      <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" ht="15.6" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" ht="16.35" spans="1:2">
-      <c r="A30" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" ht="15.6" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" ht="16.35" spans="1:2">
-      <c r="A31" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" ht="15.6" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" ht="16.35" spans="1:2">
-      <c r="A32" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" ht="15.6" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" ht="16.35" spans="1:2">
-      <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" ht="15.6" spans="1:2">
+      <c r="A33" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" ht="16.35" spans="1:2">
-      <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" ht="15.6" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" ht="16.35" spans="1:2">
-      <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" ht="15.6" spans="1:2">
+      <c r="A35" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" ht="16.35" spans="1:2">
-      <c r="A36" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" ht="15.6" spans="1:2">
+      <c r="A36" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" ht="16.35" spans="1:2">
-      <c r="A37" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" ht="15.6" spans="1:2">
+      <c r="A37" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" ht="16.35" spans="1:2">
-      <c r="A38" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="4" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>